<commit_message>
feat: improved parser.py so xlsx parser support blank padding now
Signed-off-by: Hz6826 <hz_2007@qq.com>
</commit_message>
<xml_diff>
--- a/.test/config/seat_table.xlsx
+++ b/.test/config/seat_table.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\pySeatShuffle\.test\config\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DB17F2-EE28-49A5-A28E-1D93EC263E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="15795" windowHeight="11655"/>
   </bookViews>
   <sheets>
     <sheet name="seat_table" sheetId="1" r:id="rId1"/>
@@ -33,19 +27,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="4">
   <si>
     <t>测试座位表</t>
   </si>
   <si>
     <t>{{SEAT}}</t>
   </si>
+  <si>
+    <t>生成时间</t>
+  </si>
+  <si>
+    <t>{{GENERATED_TIME}}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,21 +68,345 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -112,204 +442,349 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF7F7F7F"/>
       </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
         </patternFill>
       </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
+        <b val="1"/>
         <color theme="1"/>
       </font>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <border>
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <top style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79995117038483843"/>
-          <bgColor theme="4" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <color theme="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <border>
@@ -320,7 +795,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="0"/>
       </font>
       <fill>
@@ -348,40 +823,154 @@
           <color theme="4"/>
         </bottom>
         <horizontal style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
+          <color theme="4" tint="0.399975585192419"/>
         </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
       </border>
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
     <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
     <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
-      <tableStyleElement type="headerRow" dxfId="9"/>
-      <tableStyleElement type="totalRow" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="5"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="4"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="3"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="2"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="1"/>
-      <tableStyleElement type="pageFieldValues" dxfId="0"/>
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -639,222 +1228,233 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="B1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="42" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="42" customHeight="1" spans="2:12">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="2:12">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="L2" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    <row r="3" spans="2:12">
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
+    <row r="4" spans="2:12">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="L4" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="5" spans="2:12">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="I5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="L5" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="6" spans="2:12">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="I6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="L6" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="7" spans="2:12">
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="I7" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="L7" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
+    <row r="8" spans="2:12">
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="I8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>1</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="11:12">
+      <c r="K10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L10" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B1:L1"/>
   </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>